<commit_message>
Soy la secretaria del lab
</commit_message>
<xml_diff>
--- a/Finanzas/Becas.xlsx
+++ b/Finanzas/Becas.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>L I C E N C I A T U R A</t>
   </si>
@@ -78,6 +79,18 @@
   </si>
   <si>
     <t>Karina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t>INGENIERIA</t>
+  </si>
+  <si>
+    <t>PSICOLOGIA</t>
+  </si>
+  <si>
+    <t>Mau</t>
   </si>
 </sst>
 </file>
@@ -115,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +180,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -183,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -195,12 +256,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFFFCC99"/>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -477,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="A6:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,4 +733,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11">
+        <v>104000</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="19"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
+        <f>SUM(B10,C10,D10,G10)</f>
+        <v>65760</v>
+      </c>
+      <c r="F3" s="18">
+        <f>C2-E3</f>
+        <v>38240</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="14">
+        <f>SUM(F10,E10)</f>
+        <v>84930</v>
+      </c>
+      <c r="I3" s="19">
+        <f>C2-H3</f>
+        <v>19070</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <f>D8-950</f>
+        <v>1315</v>
+      </c>
+      <c r="C8" s="16">
+        <f>D8-1000</f>
+        <v>1265</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2265</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2831</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2831</v>
+      </c>
+      <c r="G8" s="6">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <f>B8*(SUM(B11:B211))</f>
+        <v>7890</v>
+      </c>
+      <c r="C10" s="16">
+        <f>C8*(SUM(C11:C211))</f>
+        <v>7590</v>
+      </c>
+      <c r="D10" s="2">
+        <f>D8*(SUM(D11:D212))</f>
+        <v>27180</v>
+      </c>
+      <c r="E10" s="2">
+        <f>E8*(SUM(E11:E212))</f>
+        <v>50958</v>
+      </c>
+      <c r="F10" s="2">
+        <f>F8*(SUM(F11:F212))</f>
+        <v>33972</v>
+      </c>
+      <c r="G10" s="6">
+        <f>G8*SUM(G11:G212)</f>
+        <v>23100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="13">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>